<commit_message>
added tests to ExcelReaderPairedDataTests
fixed isPairedData in ExcelReader
</commit_message>
<xml_diff>
--- a/DSSExcelTests/test-files/indexedPairedData1.xlsx
+++ b/DSSExcelTests/test-files/indexedPairedData1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DSSExcelPlugin\DSSExcelTests\test-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF73D59-8287-46B9-AFF3-C5ABC657E136}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53291627-DF2E-486F-AB83-D934DCEF4A48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="765" yWindow="6585" windowWidth="15330" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
-  <si>
-    <t>Labels</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t/>
   </si>
@@ -41,15 +38,26 @@
   </si>
   <si>
     <t>linear</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>Y2</t>
+  </si>
+  <si>
+    <t>Y3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -80,10 +88,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -403,7 +410,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -414,70 +423,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>1</v>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>1</v>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="2">
-        <v>1</v>
+      <c r="B4" s="1">
+        <v>10</v>
       </c>
       <c r="C4" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1">
-        <v>20</v>
-      </c>
-      <c r="E4" s="1">
         <v>30</v>
       </c>
     </row>
@@ -485,16 +489,13 @@
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="2">
-        <v>2</v>
+      <c r="B5" s="1">
+        <v>11</v>
       </c>
       <c r="C5" s="1">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1">
-        <v>22</v>
-      </c>
-      <c r="E5" s="1">
         <v>33</v>
       </c>
     </row>
@@ -502,16 +503,13 @@
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" s="2">
-        <v>3</v>
+      <c r="B6" s="1">
+        <v>12</v>
       </c>
       <c r="C6" s="1">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1">
-        <v>24</v>
-      </c>
-      <c r="E6" s="1">
         <v>36</v>
       </c>
     </row>
@@ -519,16 +517,13 @@
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" s="2">
-        <v>4</v>
+      <c r="B7" s="1">
+        <v>13</v>
       </c>
       <c r="C7" s="1">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1">
-        <v>26</v>
-      </c>
-      <c r="E7" s="1">
         <v>39</v>
       </c>
     </row>
@@ -536,16 +531,13 @@
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8" s="2">
-        <v>5</v>
+      <c r="B8" s="1">
+        <v>14</v>
       </c>
       <c r="C8" s="1">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D8" s="1">
-        <v>28</v>
-      </c>
-      <c r="E8" s="1">
         <v>42</v>
       </c>
     </row>
@@ -553,16 +545,13 @@
       <c r="A9">
         <v>6</v>
       </c>
-      <c r="B9" s="2">
-        <v>6</v>
+      <c r="B9" s="1">
+        <v>15</v>
       </c>
       <c r="C9" s="1">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D9" s="1">
-        <v>30</v>
-      </c>
-      <c r="E9" s="1">
         <v>45</v>
       </c>
     </row>
@@ -570,16 +559,13 @@
       <c r="A10">
         <v>7</v>
       </c>
-      <c r="B10" s="2">
-        <v>7</v>
+      <c r="B10" s="1">
+        <v>16</v>
       </c>
       <c r="C10" s="1">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D10" s="1">
-        <v>32</v>
-      </c>
-      <c r="E10" s="1">
         <v>48</v>
       </c>
     </row>

</xml_diff>